<commit_message>
relative entity was changed
</commit_message>
<xml_diff>
--- a/LMS-WhizAcademySystem.Server/UploadedFile.xlsx
+++ b/LMS-WhizAcademySystem.Server/UploadedFile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Task</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">NaN </t>
   </si>
   <si>
-    <t>Много слаб студент скоро ще го пребия</t>
+    <t>kl,</t>
   </si>
   <si>
     <t>Setting up the Environment</t>
@@ -58,7 +58,7 @@
     <t>Configure the development environment</t>
   </si>
   <si>
-    <t>S-E</t>
+    <t>NaN</t>
   </si>
   <si>
     <t>Understand Console.WriteLine()</t>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Understand Console.ReadLine()</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
   <si>
     <t>Learn about int, double, char, string, decimal, bool</t>
@@ -404,9 +401,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="0" formatCode="General"/>
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
@@ -687,10 +682,10 @@
     </row>
     <row r="6" ht="13.8">
       <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -707,10 +702,10 @@
     </row>
     <row r="7" ht="13.8">
       <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>8</v>
@@ -727,10 +722,10 @@
     </row>
     <row r="8" ht="13.8">
       <c r="A8" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>8</v>
@@ -747,10 +742,10 @@
     </row>
     <row r="9" ht="13.8">
       <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
@@ -767,10 +762,10 @@
     </row>
     <row r="10" ht="13.8">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>8</v>
@@ -787,10 +782,10 @@
     </row>
     <row r="11" ht="13.8">
       <c r="A11" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>8</v>
@@ -807,10 +802,10 @@
     </row>
     <row r="12" ht="13.8">
       <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>8</v>
@@ -827,10 +822,10 @@
     </row>
     <row r="13" ht="13.8">
       <c r="A13" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>8</v>
@@ -847,10 +842,10 @@
     </row>
     <row r="14" ht="13.8">
       <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>8</v>
@@ -867,10 +862,10 @@
     </row>
     <row r="15" ht="13.8">
       <c r="A15" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>8</v>
@@ -887,10 +882,10 @@
     </row>
     <row r="16" ht="13.8">
       <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>8</v>
@@ -907,10 +902,10 @@
     </row>
     <row r="17" ht="13.8">
       <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>8</v>
@@ -927,10 +922,10 @@
     </row>
     <row r="18" ht="13.8">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>8</v>
@@ -947,10 +942,10 @@
     </row>
     <row r="19" ht="13.8">
       <c r="A19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>8</v>
@@ -967,10 +962,10 @@
     </row>
     <row r="20" ht="13.8">
       <c r="A20" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>8</v>
@@ -987,10 +982,10 @@
     </row>
     <row r="21" ht="13.8">
       <c r="A21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>8</v>
@@ -1007,10 +1002,10 @@
     </row>
     <row r="22" ht="13.8">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>8</v>
@@ -1027,10 +1022,10 @@
     </row>
     <row r="23" ht="13.8">
       <c r="A23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>8</v>
@@ -1047,10 +1042,10 @@
     </row>
     <row r="24" ht="13.8">
       <c r="A24" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>8</v>
@@ -1067,10 +1062,10 @@
     </row>
     <row r="25" ht="13.8">
       <c r="A25" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>45</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>8</v>
@@ -1087,10 +1082,10 @@
     </row>
     <row r="26" ht="13.8">
       <c r="A26" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>8</v>
@@ -1107,10 +1102,10 @@
     </row>
     <row r="27" ht="13.8">
       <c r="A27" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>8</v>
@@ -1127,10 +1122,10 @@
     </row>
     <row r="28" ht="13.8">
       <c r="A28" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>8</v>
@@ -1147,10 +1142,10 @@
     </row>
     <row r="29" ht="13.8">
       <c r="A29" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>8</v>
@@ -1167,10 +1162,10 @@
     </row>
     <row r="30" ht="13.8">
       <c r="A30" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>8</v>
@@ -1187,10 +1182,10 @@
     </row>
     <row r="31" ht="13.8">
       <c r="A31" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>8</v>
@@ -1207,10 +1202,10 @@
     </row>
     <row r="32" ht="13.8">
       <c r="A32" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>8</v>
@@ -1227,10 +1222,10 @@
     </row>
     <row r="33" ht="13.8">
       <c r="A33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>8</v>
@@ -1247,10 +1242,10 @@
     </row>
     <row r="34" ht="13.8">
       <c r="A34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>8</v>
@@ -1267,10 +1262,10 @@
     </row>
     <row r="35" ht="13.8">
       <c r="A35" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>8</v>
@@ -1287,10 +1282,10 @@
     </row>
     <row r="36" ht="13.8">
       <c r="A36" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>8</v>
@@ -1307,10 +1302,10 @@
     </row>
     <row r="37" ht="13.8">
       <c r="A37" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>8</v>
@@ -1327,10 +1322,10 @@
     </row>
     <row r="38" ht="13.8">
       <c r="A38" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>8</v>
@@ -1347,10 +1342,10 @@
     </row>
     <row r="39" ht="13.8">
       <c r="A39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>8</v>
@@ -1367,10 +1362,10 @@
     </row>
     <row r="40" ht="13.8">
       <c r="A40" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>8</v>
@@ -1387,10 +1382,10 @@
     </row>
     <row r="41" ht="13.8">
       <c r="A41" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>69</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>8</v>
@@ -1407,10 +1402,10 @@
     </row>
     <row r="42" ht="13.8">
       <c r="A42" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>8</v>
@@ -1427,10 +1422,10 @@
     </row>
     <row r="43" ht="13.8">
       <c r="A43" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>8</v>
@@ -1447,10 +1442,10 @@
     </row>
     <row r="44" ht="13.8">
       <c r="A44" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>8</v>
@@ -1467,10 +1462,10 @@
     </row>
     <row r="45" ht="13.8">
       <c r="A45" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>8</v>
@@ -1487,10 +1482,10 @@
     </row>
     <row r="46" ht="13.8">
       <c r="A46" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>8</v>
@@ -1507,10 +1502,10 @@
     </row>
     <row r="47" ht="13.8">
       <c r="A47" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>8</v>
@@ -1527,10 +1522,10 @@
     </row>
     <row r="48" ht="13.8">
       <c r="A48" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>8</v>
@@ -1547,10 +1542,10 @@
     </row>
     <row r="49" ht="13.8">
       <c r="A49" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>8</v>
@@ -1567,10 +1562,10 @@
     </row>
     <row r="50" ht="13.8">
       <c r="A50" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>8</v>
@@ -1587,10 +1582,10 @@
     </row>
     <row r="51" ht="13.8">
       <c r="A51" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>8</v>
@@ -1607,10 +1602,10 @@
     </row>
     <row r="52" ht="13.8">
       <c r="A52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>8</v>
@@ -1627,10 +1622,10 @@
     </row>
     <row r="53" ht="13.8">
       <c r="A53" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>8</v>
@@ -1647,10 +1642,10 @@
     </row>
     <row r="54" ht="13.8">
       <c r="A54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>8</v>
@@ -1667,10 +1662,10 @@
     </row>
     <row r="55" ht="13.8">
       <c r="A55" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>8</v>
@@ -1687,10 +1682,10 @@
     </row>
     <row r="56" ht="13.8">
       <c r="A56" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>8</v>
@@ -1707,10 +1702,10 @@
     </row>
     <row r="57" ht="13.8">
       <c r="A57" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>8</v>
@@ -1727,10 +1722,10 @@
     </row>
     <row r="58" ht="13.8">
       <c r="A58" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>8</v>
@@ -1747,10 +1742,10 @@
     </row>
     <row r="59" ht="13.8">
       <c r="A59" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>8</v>
@@ -1767,10 +1762,10 @@
     </row>
     <row r="60" ht="13.8">
       <c r="A60" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>8</v>
@@ -1787,10 +1782,10 @@
     </row>
     <row r="61" ht="13.8">
       <c r="A61" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>99</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>8</v>
@@ -1807,10 +1802,10 @@
     </row>
     <row r="62" ht="13.8">
       <c r="A62" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>8</v>
@@ -1827,10 +1822,10 @@
     </row>
     <row r="63" ht="13.8">
       <c r="A63" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>8</v>
@@ -1847,10 +1842,10 @@
     </row>
     <row r="64" ht="13.8">
       <c r="A64" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>104</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>8</v>
@@ -1867,10 +1862,10 @@
     </row>
     <row r="65" ht="13.8">
       <c r="A65" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>8</v>
@@ -1887,10 +1882,10 @@
     </row>
     <row r="66" ht="13.8">
       <c r="A66" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>8</v>
@@ -1907,10 +1902,10 @@
     </row>
     <row r="67" ht="13.8">
       <c r="A67" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B67" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>109</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>8</v>
@@ -1927,10 +1922,10 @@
     </row>
     <row r="68" ht="13.8">
       <c r="A68" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>8</v>
@@ -1947,10 +1942,10 @@
     </row>
     <row r="69" ht="13.8">
       <c r="A69" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>8</v>
@@ -1967,10 +1962,10 @@
     </row>
     <row r="70" ht="13.8">
       <c r="A70" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>8</v>
@@ -1987,10 +1982,10 @@
     </row>
     <row r="71" ht="13.8">
       <c r="A71" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B71" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>8</v>
@@ -2007,10 +2002,10 @@
     </row>
     <row r="72" ht="13.8">
       <c r="A72" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>8</v>
@@ -2027,10 +2022,10 @@
     </row>
     <row r="73" ht="13.8">
       <c r="A73" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" s="7" t="s">
         <v>117</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>118</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>8</v>
@@ -2047,10 +2042,10 @@
     </row>
     <row r="74" ht="13.8">
       <c r="A74" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>8</v>
@@ -2067,10 +2062,10 @@
     </row>
     <row r="75" ht="13.8">
       <c r="A75" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>8</v>
@@ -2087,10 +2082,10 @@
     </row>
     <row r="76" ht="13.8">
       <c r="A76" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>8</v>
@@ -2107,10 +2102,10 @@
     </row>
     <row r="77" ht="13.8">
       <c r="A77" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>124</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>8</v>
@@ -2127,10 +2122,10 @@
     </row>
     <row r="78" ht="13.8">
       <c r="A78" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>8</v>

</xml_diff>